<commit_message>
Add r factor analsyis workspace and output
</commit_message>
<xml_diff>
--- a/output/FactorAnalysis.xlsx
+++ b/output/FactorAnalysis.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Google Drive\AsianBrazil\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C75D70A-D854-4452-869E-441586BD06F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82057B7-2103-4765-9270-19447754A921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="109635" yWindow="12450" windowWidth="10800" windowHeight="5700" xr2:uid="{29B5723C-62C6-49F4-9D97-29B745FB8889}"/>
+    <workbookView xWindow="86280" yWindow="4110" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29B5723C-62C6-49F4-9D97-29B745FB8889}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Stata" sheetId="1" r:id="rId1"/>
+    <sheet name="R" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Variable</t>
   </si>
@@ -85,6 +86,102 @@
   </si>
   <si>
     <t>KMO</t>
+  </si>
+  <si>
+    <t>pol1</t>
+  </si>
+  <si>
+    <t>conocim</t>
+  </si>
+  <si>
+    <t>eff2_reordered</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
+  <si>
+    <t>b6</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>b12</t>
+  </si>
+  <si>
+    <t>b13</t>
+  </si>
+  <si>
+    <t>b21</t>
+  </si>
+  <si>
+    <t>b21a</t>
+  </si>
+  <si>
+    <t>b32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b47a </t>
+  </si>
+  <si>
+    <t>Sente orgulhoso de viver no sistema político</t>
+  </si>
+  <si>
+    <t>Deve apoiar o sistema político</t>
+  </si>
+  <si>
+    <t>0,64</t>
+  </si>
+  <si>
+    <t>0,42</t>
+  </si>
+  <si>
+    <t>0,58</t>
+  </si>
+  <si>
+    <t>0,53</t>
+  </si>
+  <si>
+    <t>0,57</t>
+  </si>
+  <si>
+    <t>0,69</t>
+  </si>
+  <si>
+    <t>0,68</t>
+  </si>
+  <si>
+    <t>0,71</t>
+  </si>
+  <si>
+    <t>0,70</t>
+  </si>
+  <si>
+    <t>0,60</t>
+  </si>
+  <si>
+    <t>0,56</t>
+  </si>
+  <si>
+    <t>0,61</t>
+  </si>
+  <si>
+    <t>0,931</t>
+  </si>
+  <si>
+    <t>0,8676</t>
+  </si>
+  <si>
+    <t>0,609</t>
+  </si>
+  <si>
+    <t>0,4977</t>
   </si>
 </sst>
 </file>
@@ -438,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3AED69-352D-4570-9A7E-566DF55DCE03}">
   <dimension ref="A3:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,4 +687,221 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050183F1-BDD7-47A5-BF61-09C62C2376E3}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ouput; factor analysis and regression
</commit_message>
<xml_diff>
--- a/output/FactorAnalysis.xlsx
+++ b/output/FactorAnalysis.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Google Drive\AsianBrazil\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82057B7-2103-4765-9270-19447754A921}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0904BB-B47D-49C5-8A71-66D19BFC16F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="4110" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{29B5723C-62C6-49F4-9D97-29B745FB8889}"/>
+    <workbookView xWindow="73680" yWindow="4110" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{29B5723C-62C6-49F4-9D97-29B745FB8889}"/>
   </bookViews>
   <sheets>
     <sheet name="Stata" sheetId="1" r:id="rId1"/>
     <sheet name="R" sheetId="2" r:id="rId2"/>
+    <sheet name="R_PolyChoric" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
   <si>
     <t>Variable</t>
   </si>
@@ -182,6 +183,39 @@
   </si>
   <si>
     <t>0,4977</t>
+  </si>
+  <si>
+    <t>0,5524</t>
+  </si>
+  <si>
+    <t>0,59</t>
+  </si>
+  <si>
+    <t>0,44</t>
+  </si>
+  <si>
+    <t>0,35</t>
+  </si>
+  <si>
+    <t>0,45</t>
+  </si>
+  <si>
+    <t>0,73</t>
+  </si>
+  <si>
+    <t>0,74</t>
+  </si>
+  <si>
+    <t>0,46</t>
+  </si>
+  <si>
+    <t>0,75</t>
+  </si>
+  <si>
+    <t>0,78</t>
+  </si>
+  <si>
+    <t>0,66</t>
   </si>
 </sst>
 </file>
@@ -205,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -213,12 +247,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +839,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050183F1-BDD7-47A5-BF61-09C62C2376E3}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,201 +851,460 @@
     <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2">
+        <v>39</v>
+      </c>
+      <c r="D18" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDDC6B7-24A7-4D8F-A217-6B506E1F29BA}">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="4"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
+      <c r="C5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
+      <c r="C6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
+      <c r="C7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
-      </c>
+      <c r="C8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
+      <c r="C9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
+      <c r="C11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
+      <c r="C12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
+      <c r="C13" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>36</v>
+      <c r="C14" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
-        <v>34</v>
+      <c r="C15" s="2"/>
+      <c r="D15" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>35</v>
+      <c r="C16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17">
-        <v>39</v>
-      </c>
-      <c r="D17">
-        <v>31</v>
+      <c r="C17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D18" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>